<commit_message>
update for problem list
</commit_message>
<xml_diff>
--- a/0_docs/CheckListForm_1week.xlsx
+++ b/0_docs/CheckListForm_1week.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOJINYOU\Dropbox\MJU\Coin\2.study\21_1\Study-21-1-codingTest\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOJINYOU\Dropbox\MJU\Coin\2.study\21_1\Study-21-1-codingTest\dojinyou\code_1week\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97C278E-49EC-404F-A0E9-CD5F07112420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDA0738-81EC-44CF-813C-C61D7726B937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2683A084-5E1C-45DB-8DAE-141C5F5642CD}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{2683A084-5E1C-45DB-8DAE-141C5F5642CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="63">
   <si>
     <t>이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,6 +105,186 @@
   <si>
     <t>시작 후
 1시간 경과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/2920</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21.03.04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>블랙잭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/2798</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/1920</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/10828</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/9012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>괄호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/10799</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쇠막대기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/5397</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>키로거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/1966</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프린터 큐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/10845</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>큐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/10866</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>덱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/10808</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알파벳 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deck</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Queue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/10809</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>알파벳 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/10820</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>문자열 분석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/2743</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단어 길이 재기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/11655</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROT13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/10824</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네 수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/11656</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>접미사 배열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linked-list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/1406</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에디터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/1158</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요세푸스 문제</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -112,7 +292,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +326,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -543,18 +732,108 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,102 +843,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -971,16 +1170,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA290B9-D938-4FB9-A2F0-C9496544FB19}">
-  <dimension ref="B1:F26"/>
+  <dimension ref="B1:F230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:F12"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D221" sqref="D221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="3.296875" customWidth="1"/>
-    <col min="2" max="2" width="9.796875" customWidth="1"/>
+    <col min="2" max="2" width="10.09765625" customWidth="1"/>
     <col min="3" max="3" width="4.59765625" customWidth="1"/>
     <col min="4" max="4" width="39.09765625" customWidth="1"/>
     <col min="5" max="5" width="14.3984375" customWidth="1"/>
@@ -989,257 +1188,2451 @@
   <sheetData>
     <row r="1" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="33" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="32" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+    <row r="3" spans="2:6" s="8" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="22" t="s">
+      <c r="C7" s="35"/>
+      <c r="D7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="24"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="17"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="18" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="22" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="24"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="14" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="17"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="18" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
     </row>
     <row r="15" spans="2:6" ht="7.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="16" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
+      <c r="C16" s="27"/>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B19" s="35" t="s">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="22" t="s">
+      <c r="C19" s="35"/>
+      <c r="D19" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14" t="s">
+      <c r="B22" s="20"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="17"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="18" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="25"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="22" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="14" t="s">
+      <c r="B25" s="20"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="16"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="17"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="18" t="s">
+      <c r="B26" s="21"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B28" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="27"/>
+      <c r="D28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B29" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B30" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B31" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="35"/>
+      <c r="D31" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="30"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B32" s="20"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B33" s="20"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B34" s="20"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="21"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="24"/>
+      <c r="F35" s="25"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B36" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B37" s="20"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="12"/>
+      <c r="F37" s="13"/>
+    </row>
+    <row r="38" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B38" s="21"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="24"/>
+      <c r="F38" s="25"/>
+    </row>
+    <row r="39" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B40" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B41" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B42" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B43" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="35"/>
+      <c r="D43" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="30"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B44" s="20"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B45" s="20"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="12"/>
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B46" s="20"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B47" s="21"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="24"/>
+      <c r="F47" s="25"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B48" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="29"/>
+      <c r="F48" s="30"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B49" s="20"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="12"/>
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="21"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="24"/>
+      <c r="F50" s="25"/>
+    </row>
+    <row r="51" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B52" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="27"/>
+      <c r="D52" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="18"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B55" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="35"/>
+      <c r="D55" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="29"/>
+      <c r="F55" s="30"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B56" s="20"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="12"/>
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B57" s="20"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="12"/>
+      <c r="F57" s="13"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B58" s="20"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="12"/>
+      <c r="F58" s="13"/>
+    </row>
+    <row r="59" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B59" s="21"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="24"/>
+      <c r="F59" s="25"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B60" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="29"/>
+      <c r="F60" s="30"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B61" s="20"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="12"/>
+      <c r="F61" s="13"/>
+    </row>
+    <row r="62" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="21"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="24"/>
+      <c r="F62" s="25"/>
+    </row>
+    <row r="63" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B64" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="27"/>
+      <c r="D64" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B65" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="15"/>
+      <c r="D65" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B66" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="18"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B67" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="35"/>
+      <c r="D67" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="29"/>
+      <c r="F67" s="30"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B68" s="20"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="12"/>
+      <c r="F68" s="13"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B69" s="20"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="12"/>
+      <c r="F69" s="13"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B70" s="20"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" s="12"/>
+      <c r="F70" s="13"/>
+    </row>
+    <row r="71" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B71" s="21"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="24"/>
+      <c r="F71" s="25"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B72" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E72" s="29"/>
+      <c r="F72" s="30"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B73" s="20"/>
+      <c r="C73" s="37"/>
+      <c r="D73" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" s="12"/>
+      <c r="F73" s="13"/>
+    </row>
+    <row r="74" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B74" s="21"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="24"/>
+      <c r="F74" s="25"/>
+    </row>
+    <row r="75" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B76" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="27"/>
+      <c r="D76" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B77" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C77" s="15"/>
+      <c r="D77" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B78" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="18"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B79" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="35"/>
+      <c r="D79" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="29"/>
+      <c r="F79" s="30"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B80" s="20"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="12"/>
+      <c r="F80" s="13"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B81" s="20"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="12"/>
+      <c r="F81" s="13"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B82" s="20"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="12"/>
+      <c r="F82" s="13"/>
+    </row>
+    <row r="83" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B83" s="21"/>
+      <c r="C83" s="36"/>
+      <c r="D83" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="24"/>
+      <c r="F83" s="25"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B84" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E84" s="29"/>
+      <c r="F84" s="30"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B85" s="20"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E85" s="12"/>
+      <c r="F85" s="13"/>
+    </row>
+    <row r="86" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B86" s="21"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86" s="24"/>
+      <c r="F86" s="25"/>
+    </row>
+    <row r="87" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B88" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" s="27"/>
+      <c r="D88" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B89" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C89" s="15"/>
+      <c r="D89" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B90" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="17"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="18"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B91" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C91" s="35"/>
+      <c r="D91" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="29"/>
+      <c r="F91" s="30"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B92" s="20"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E92" s="12"/>
+      <c r="F92" s="13"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B93" s="20"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E93" s="12"/>
+      <c r="F93" s="13"/>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B94" s="20"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="12"/>
+      <c r="F94" s="13"/>
+    </row>
+    <row r="95" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B95" s="21"/>
+      <c r="C95" s="36"/>
+      <c r="D95" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" s="24"/>
+      <c r="F95" s="25"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B96" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E96" s="29"/>
+      <c r="F96" s="30"/>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B97" s="20"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97" s="12"/>
+      <c r="F97" s="13"/>
+    </row>
+    <row r="98" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B98" s="21"/>
+      <c r="C98" s="36"/>
+      <c r="D98" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E98" s="24"/>
+      <c r="F98" s="25"/>
+    </row>
+    <row r="99" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B100" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="27"/>
+      <c r="D100" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B101" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="15"/>
+      <c r="D101" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B102" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="17"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="18"/>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B103" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103" s="35"/>
+      <c r="D103" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" s="29"/>
+      <c r="F103" s="30"/>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B104" s="20"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104" s="12"/>
+      <c r="F104" s="13"/>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B105" s="20"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E105" s="12"/>
+      <c r="F105" s="13"/>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B106" s="20"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="12"/>
+      <c r="F106" s="13"/>
+    </row>
+    <row r="107" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B107" s="21"/>
+      <c r="C107" s="36"/>
+      <c r="D107" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E107" s="24"/>
+      <c r="F107" s="25"/>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B108" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E108" s="29"/>
+      <c r="F108" s="30"/>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B109" s="20"/>
+      <c r="C109" s="37"/>
+      <c r="D109" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E109" s="12"/>
+      <c r="F109" s="13"/>
+    </row>
+    <row r="110" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B110" s="21"/>
+      <c r="C110" s="36"/>
+      <c r="D110" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E110" s="24"/>
+      <c r="F110" s="25"/>
+    </row>
+    <row r="111" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B112" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C112" s="27"/>
+      <c r="D112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B113" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C113" s="15"/>
+      <c r="D113" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B114" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" s="17"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="18"/>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B115" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115" s="35"/>
+      <c r="D115" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" s="29"/>
+      <c r="F115" s="30"/>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B116" s="20"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" s="12"/>
+      <c r="F116" s="13"/>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B117" s="20"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" s="12"/>
+      <c r="F117" s="13"/>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B118" s="20"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118" s="12"/>
+      <c r="F118" s="13"/>
+    </row>
+    <row r="119" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B119" s="21"/>
+      <c r="C119" s="36"/>
+      <c r="D119" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E119" s="24"/>
+      <c r="F119" s="25"/>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B120" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C120" s="1"/>
+      <c r="D120" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E120" s="29"/>
+      <c r="F120" s="30"/>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B121" s="20"/>
+      <c r="C121" s="37"/>
+      <c r="D121" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E121" s="12"/>
+      <c r="F121" s="13"/>
+    </row>
+    <row r="122" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B122" s="21"/>
+      <c r="C122" s="36"/>
+      <c r="D122" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E122" s="24"/>
+      <c r="F122" s="25"/>
+    </row>
+    <row r="123" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B124" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C124" s="27"/>
+      <c r="D124" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B125" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C125" s="15"/>
+      <c r="D125" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F125" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B126" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" s="17"/>
+      <c r="D126" s="17"/>
+      <c r="E126" s="17"/>
+      <c r="F126" s="18"/>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B127" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C127" s="35"/>
+      <c r="D127" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E127" s="29"/>
+      <c r="F127" s="30"/>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B128" s="20"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E128" s="12"/>
+      <c r="F128" s="13"/>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B129" s="20"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E129" s="12"/>
+      <c r="F129" s="13"/>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B130" s="20"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E130" s="12"/>
+      <c r="F130" s="13"/>
+    </row>
+    <row r="131" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B131" s="21"/>
+      <c r="C131" s="36"/>
+      <c r="D131" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E131" s="24"/>
+      <c r="F131" s="25"/>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B132" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132" s="1"/>
+      <c r="D132" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E132" s="29"/>
+      <c r="F132" s="30"/>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B133" s="20"/>
+      <c r="C133" s="37"/>
+      <c r="D133" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E133" s="12"/>
+      <c r="F133" s="13"/>
+    </row>
+    <row r="134" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B134" s="21"/>
+      <c r="C134" s="36"/>
+      <c r="D134" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E134" s="24"/>
+      <c r="F134" s="25"/>
+    </row>
+    <row r="135" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B136" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136" s="27"/>
+      <c r="D136" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B137" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" s="15"/>
+      <c r="D137" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B138" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138" s="17"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="18"/>
+    </row>
+    <row r="139" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B139" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C139" s="35"/>
+      <c r="D139" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" s="29"/>
+      <c r="F139" s="30"/>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B140" s="20"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E140" s="12"/>
+      <c r="F140" s="13"/>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B141" s="20"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E141" s="12"/>
+      <c r="F141" s="13"/>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B142" s="20"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E142" s="12"/>
+      <c r="F142" s="13"/>
+    </row>
+    <row r="143" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B143" s="21"/>
+      <c r="C143" s="36"/>
+      <c r="D143" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143" s="24"/>
+      <c r="F143" s="25"/>
+    </row>
+    <row r="144" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B144" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144" s="1"/>
+      <c r="D144" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E144" s="29"/>
+      <c r="F144" s="30"/>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B145" s="20"/>
+      <c r="C145" s="37"/>
+      <c r="D145" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E145" s="12"/>
+      <c r="F145" s="13"/>
+    </row>
+    <row r="146" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B146" s="21"/>
+      <c r="C146" s="36"/>
+      <c r="D146" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E146" s="24"/>
+      <c r="F146" s="25"/>
+    </row>
+    <row r="147" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B148" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C148" s="27"/>
+      <c r="D148" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B149" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C149" s="15"/>
+      <c r="D149" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F149" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="150" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B150" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150" s="17"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="18"/>
+    </row>
+    <row r="151" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B151" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C151" s="35"/>
+      <c r="D151" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E151" s="29"/>
+      <c r="F151" s="30"/>
+    </row>
+    <row r="152" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B152" s="20"/>
+      <c r="C152" s="5"/>
+      <c r="D152" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E152" s="12"/>
+      <c r="F152" s="13"/>
+    </row>
+    <row r="153" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B153" s="20"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E153" s="12"/>
+      <c r="F153" s="13"/>
+    </row>
+    <row r="154" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B154" s="20"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E154" s="12"/>
+      <c r="F154" s="13"/>
+    </row>
+    <row r="155" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B155" s="21"/>
+      <c r="C155" s="36"/>
+      <c r="D155" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E155" s="24"/>
+      <c r="F155" s="25"/>
+    </row>
+    <row r="156" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B156" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C156" s="1"/>
+      <c r="D156" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E156" s="29"/>
+      <c r="F156" s="30"/>
+    </row>
+    <row r="157" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B157" s="20"/>
+      <c r="C157" s="37"/>
+      <c r="D157" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E157" s="12"/>
+      <c r="F157" s="13"/>
+    </row>
+    <row r="158" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B158" s="21"/>
+      <c r="C158" s="36"/>
+      <c r="D158" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E158" s="24"/>
+      <c r="F158" s="25"/>
+    </row>
+    <row r="159" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="160" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B160" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160" s="27"/>
+      <c r="D160" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="161" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B161" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C161" s="15"/>
+      <c r="D161" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F161" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="162" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B162" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C162" s="17"/>
+      <c r="D162" s="17"/>
+      <c r="E162" s="17"/>
+      <c r="F162" s="18"/>
+    </row>
+    <row r="163" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B163" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C163" s="35"/>
+      <c r="D163" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E163" s="29"/>
+      <c r="F163" s="30"/>
+    </row>
+    <row r="164" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B164" s="20"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E164" s="12"/>
+      <c r="F164" s="13"/>
+    </row>
+    <row r="165" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B165" s="20"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E165" s="12"/>
+      <c r="F165" s="13"/>
+    </row>
+    <row r="166" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B166" s="20"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E166" s="12"/>
+      <c r="F166" s="13"/>
+    </row>
+    <row r="167" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B167" s="21"/>
+      <c r="C167" s="36"/>
+      <c r="D167" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E167" s="24"/>
+      <c r="F167" s="25"/>
+    </row>
+    <row r="168" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B168" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168" s="1"/>
+      <c r="D168" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E168" s="29"/>
+      <c r="F168" s="30"/>
+    </row>
+    <row r="169" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B169" s="20"/>
+      <c r="C169" s="37"/>
+      <c r="D169" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E169" s="12"/>
+      <c r="F169" s="13"/>
+    </row>
+    <row r="170" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B170" s="21"/>
+      <c r="C170" s="36"/>
+      <c r="D170" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E170" s="24"/>
+      <c r="F170" s="25"/>
+    </row>
+    <row r="171" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="172" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B172" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C172" s="27"/>
+      <c r="D172" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F172" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="173" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B173" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C173" s="15"/>
+      <c r="D173" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F173" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="174" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B174" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174" s="17"/>
+      <c r="D174" s="17"/>
+      <c r="E174" s="17"/>
+      <c r="F174" s="18"/>
+    </row>
+    <row r="175" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B175" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C175" s="35"/>
+      <c r="D175" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E175" s="29"/>
+      <c r="F175" s="30"/>
+    </row>
+    <row r="176" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B176" s="20"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E176" s="12"/>
+      <c r="F176" s="13"/>
+    </row>
+    <row r="177" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B177" s="20"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E177" s="12"/>
+      <c r="F177" s="13"/>
+    </row>
+    <row r="178" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B178" s="20"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E178" s="12"/>
+      <c r="F178" s="13"/>
+    </row>
+    <row r="179" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B179" s="21"/>
+      <c r="C179" s="36"/>
+      <c r="D179" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E179" s="24"/>
+      <c r="F179" s="25"/>
+    </row>
+    <row r="180" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B180" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180" s="1"/>
+      <c r="D180" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E180" s="29"/>
+      <c r="F180" s="30"/>
+    </row>
+    <row r="181" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B181" s="20"/>
+      <c r="C181" s="37"/>
+      <c r="D181" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E181" s="12"/>
+      <c r="F181" s="13"/>
+    </row>
+    <row r="182" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B182" s="21"/>
+      <c r="C182" s="36"/>
+      <c r="D182" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E182" s="24"/>
+      <c r="F182" s="25"/>
+    </row>
+    <row r="183" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="184" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B184" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C184" s="27"/>
+      <c r="D184" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="185" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B185" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C185" s="15"/>
+      <c r="D185" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F185" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="186" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B186" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C186" s="17"/>
+      <c r="D186" s="17"/>
+      <c r="E186" s="17"/>
+      <c r="F186" s="18"/>
+    </row>
+    <row r="187" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B187" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C187" s="35"/>
+      <c r="D187" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E187" s="29"/>
+      <c r="F187" s="30"/>
+    </row>
+    <row r="188" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B188" s="20"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E188" s="12"/>
+      <c r="F188" s="13"/>
+    </row>
+    <row r="189" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B189" s="20"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E189" s="12"/>
+      <c r="F189" s="13"/>
+    </row>
+    <row r="190" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B190" s="20"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E190" s="12"/>
+      <c r="F190" s="13"/>
+    </row>
+    <row r="191" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B191" s="21"/>
+      <c r="C191" s="36"/>
+      <c r="D191" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E191" s="24"/>
+      <c r="F191" s="25"/>
+    </row>
+    <row r="192" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B192" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192" s="1"/>
+      <c r="D192" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E192" s="29"/>
+      <c r="F192" s="30"/>
+    </row>
+    <row r="193" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B193" s="20"/>
+      <c r="C193" s="37"/>
+      <c r="D193" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E193" s="12"/>
+      <c r="F193" s="13"/>
+    </row>
+    <row r="194" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B194" s="21"/>
+      <c r="C194" s="36"/>
+      <c r="D194" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E194" s="24"/>
+      <c r="F194" s="25"/>
+    </row>
+    <row r="195" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="196" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B196" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C196" s="27"/>
+      <c r="D196" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F196" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="197" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B197" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C197" s="15"/>
+      <c r="D197" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F197" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="198" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B198" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C198" s="17"/>
+      <c r="D198" s="17"/>
+      <c r="E198" s="17"/>
+      <c r="F198" s="18"/>
+    </row>
+    <row r="199" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B199" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C199" s="35"/>
+      <c r="D199" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E199" s="29"/>
+      <c r="F199" s="30"/>
+    </row>
+    <row r="200" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B200" s="20"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E200" s="12"/>
+      <c r="F200" s="13"/>
+    </row>
+    <row r="201" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B201" s="20"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E201" s="12"/>
+      <c r="F201" s="13"/>
+    </row>
+    <row r="202" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B202" s="20"/>
+      <c r="C202" s="5"/>
+      <c r="D202" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E202" s="12"/>
+      <c r="F202" s="13"/>
+    </row>
+    <row r="203" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B203" s="21"/>
+      <c r="C203" s="36"/>
+      <c r="D203" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E203" s="24"/>
+      <c r="F203" s="25"/>
+    </row>
+    <row r="204" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B204" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C204" s="1"/>
+      <c r="D204" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E204" s="29"/>
+      <c r="F204" s="30"/>
+    </row>
+    <row r="205" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B205" s="20"/>
+      <c r="C205" s="37"/>
+      <c r="D205" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E205" s="12"/>
+      <c r="F205" s="13"/>
+    </row>
+    <row r="206" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B206" s="21"/>
+      <c r="C206" s="36"/>
+      <c r="D206" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E206" s="24"/>
+      <c r="F206" s="25"/>
+    </row>
+    <row r="207" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="208" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B208" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C208" s="27"/>
+      <c r="D208" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F208" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B209" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C209" s="15"/>
+      <c r="D209" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F209" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="210" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B210" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C210" s="17"/>
+      <c r="D210" s="17"/>
+      <c r="E210" s="17"/>
+      <c r="F210" s="18"/>
+    </row>
+    <row r="211" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B211" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C211" s="35"/>
+      <c r="D211" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E211" s="29"/>
+      <c r="F211" s="30"/>
+    </row>
+    <row r="212" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B212" s="20"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E212" s="12"/>
+      <c r="F212" s="13"/>
+    </row>
+    <row r="213" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B213" s="20"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E213" s="12"/>
+      <c r="F213" s="13"/>
+    </row>
+    <row r="214" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B214" s="20"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E214" s="12"/>
+      <c r="F214" s="13"/>
+    </row>
+    <row r="215" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B215" s="21"/>
+      <c r="C215" s="36"/>
+      <c r="D215" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E215" s="24"/>
+      <c r="F215" s="25"/>
+    </row>
+    <row r="216" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B216" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C216" s="1"/>
+      <c r="D216" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E216" s="29"/>
+      <c r="F216" s="30"/>
+    </row>
+    <row r="217" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B217" s="20"/>
+      <c r="C217" s="37"/>
+      <c r="D217" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E217" s="12"/>
+      <c r="F217" s="13"/>
+    </row>
+    <row r="218" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B218" s="21"/>
+      <c r="C218" s="36"/>
+      <c r="D218" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E218" s="24"/>
+      <c r="F218" s="25"/>
+    </row>
+    <row r="219" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="220" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B220" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C220" s="27"/>
+      <c r="D220" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F220" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="221" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B221" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C221" s="15"/>
+      <c r="D221" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E221" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F221" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="222" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B222" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C222" s="17"/>
+      <c r="D222" s="17"/>
+      <c r="E222" s="17"/>
+      <c r="F222" s="18"/>
+    </row>
+    <row r="223" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B223" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C223" s="35"/>
+      <c r="D223" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E223" s="29"/>
+      <c r="F223" s="30"/>
+    </row>
+    <row r="224" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B224" s="20"/>
+      <c r="C224" s="5"/>
+      <c r="D224" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E224" s="12"/>
+      <c r="F224" s="13"/>
+    </row>
+    <row r="225" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B225" s="20"/>
+      <c r="C225" s="5"/>
+      <c r="D225" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E225" s="12"/>
+      <c r="F225" s="13"/>
+    </row>
+    <row r="226" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B226" s="20"/>
+      <c r="C226" s="5"/>
+      <c r="D226" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E226" s="12"/>
+      <c r="F226" s="13"/>
+    </row>
+    <row r="227" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B227" s="21"/>
+      <c r="C227" s="36"/>
+      <c r="D227" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E227" s="24"/>
+      <c r="F227" s="25"/>
+    </row>
+    <row r="228" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B228" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C228" s="1"/>
+      <c r="D228" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E228" s="29"/>
+      <c r="F228" s="30"/>
+    </row>
+    <row r="229" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B229" s="20"/>
+      <c r="C229" s="37"/>
+      <c r="D229" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E229" s="12"/>
+      <c r="F229" s="13"/>
+    </row>
+    <row r="230" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B230" s="21"/>
+      <c r="C230" s="36"/>
+      <c r="D230" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E230" s="24"/>
+      <c r="F230" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
+  <mergeCells count="248">
+    <mergeCell ref="B228:B230"/>
+    <mergeCell ref="D228:F228"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="B221:C221"/>
+    <mergeCell ref="B222:F222"/>
+    <mergeCell ref="B223:B227"/>
+    <mergeCell ref="D223:F223"/>
+    <mergeCell ref="D224:F224"/>
+    <mergeCell ref="D225:F225"/>
+    <mergeCell ref="D226:F226"/>
+    <mergeCell ref="D227:F227"/>
+    <mergeCell ref="B216:B218"/>
+    <mergeCell ref="D216:F216"/>
+    <mergeCell ref="D217:F217"/>
+    <mergeCell ref="D218:F218"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="B209:C209"/>
+    <mergeCell ref="B210:F210"/>
+    <mergeCell ref="B211:B215"/>
+    <mergeCell ref="D211:F211"/>
+    <mergeCell ref="D212:F212"/>
+    <mergeCell ref="D213:F213"/>
+    <mergeCell ref="D214:F214"/>
+    <mergeCell ref="D215:F215"/>
+    <mergeCell ref="B204:B206"/>
+    <mergeCell ref="D204:F204"/>
+    <mergeCell ref="D205:F205"/>
+    <mergeCell ref="D206:F206"/>
+    <mergeCell ref="B208:C208"/>
+    <mergeCell ref="B197:C197"/>
+    <mergeCell ref="B198:F198"/>
+    <mergeCell ref="B199:B203"/>
+    <mergeCell ref="D199:F199"/>
+    <mergeCell ref="D200:F200"/>
+    <mergeCell ref="D201:F201"/>
+    <mergeCell ref="D202:F202"/>
+    <mergeCell ref="D203:F203"/>
+    <mergeCell ref="B192:B194"/>
+    <mergeCell ref="D192:F192"/>
+    <mergeCell ref="D193:F193"/>
+    <mergeCell ref="D194:F194"/>
+    <mergeCell ref="B196:C196"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:B191"/>
+    <mergeCell ref="D187:F187"/>
+    <mergeCell ref="D188:F188"/>
+    <mergeCell ref="D189:F189"/>
+    <mergeCell ref="D190:F190"/>
+    <mergeCell ref="D191:F191"/>
+    <mergeCell ref="B180:B182"/>
+    <mergeCell ref="D180:F180"/>
+    <mergeCell ref="D181:F181"/>
+    <mergeCell ref="D182:F182"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:B179"/>
+    <mergeCell ref="D175:F175"/>
+    <mergeCell ref="D176:F176"/>
+    <mergeCell ref="D177:F177"/>
+    <mergeCell ref="D178:F178"/>
+    <mergeCell ref="D179:F179"/>
+    <mergeCell ref="B168:B170"/>
+    <mergeCell ref="D168:F168"/>
+    <mergeCell ref="D169:F169"/>
+    <mergeCell ref="D170:F170"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B163:B167"/>
+    <mergeCell ref="D163:F163"/>
+    <mergeCell ref="D164:F164"/>
+    <mergeCell ref="D165:F165"/>
+    <mergeCell ref="D166:F166"/>
+    <mergeCell ref="D167:F167"/>
+    <mergeCell ref="B156:B158"/>
+    <mergeCell ref="D156:F156"/>
+    <mergeCell ref="D157:F157"/>
+    <mergeCell ref="D158:F158"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:B155"/>
+    <mergeCell ref="D151:F151"/>
+    <mergeCell ref="D152:F152"/>
+    <mergeCell ref="D153:F153"/>
+    <mergeCell ref="D154:F154"/>
+    <mergeCell ref="D155:F155"/>
+    <mergeCell ref="B144:B146"/>
+    <mergeCell ref="D144:F144"/>
+    <mergeCell ref="D145:F145"/>
+    <mergeCell ref="D146:F146"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:B143"/>
+    <mergeCell ref="D139:F139"/>
+    <mergeCell ref="D140:F140"/>
+    <mergeCell ref="D141:F141"/>
+    <mergeCell ref="D142:F142"/>
+    <mergeCell ref="D143:F143"/>
+    <mergeCell ref="B132:B134"/>
+    <mergeCell ref="D132:F132"/>
+    <mergeCell ref="D133:F133"/>
+    <mergeCell ref="D134:F134"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:B131"/>
+    <mergeCell ref="D127:F127"/>
+    <mergeCell ref="D128:F128"/>
+    <mergeCell ref="D129:F129"/>
+    <mergeCell ref="D130:F130"/>
+    <mergeCell ref="D131:F131"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="D122:F122"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:B119"/>
+    <mergeCell ref="D115:F115"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="D108:F108"/>
+    <mergeCell ref="D109:F109"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:B107"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="B96:B98"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D97:F97"/>
+    <mergeCell ref="D98:F98"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B4:C4"/>
@@ -1252,8 +3645,44 @@
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{2E65E543-8E67-4FF0-AE0C-07D6C31BA50B}"/>
+    <hyperlink ref="D17" r:id="rId2" xr:uid="{BB544B9E-2924-4478-8C38-79DFD09D5CCE}"/>
+    <hyperlink ref="D29" r:id="rId3" xr:uid="{CB1D523D-1CDC-4E06-B95B-0503B7530E20}"/>
+    <hyperlink ref="D41" r:id="rId4" xr:uid="{FD68BCE2-64E2-45F3-905D-47426983F315}"/>
+    <hyperlink ref="D53" r:id="rId5" xr:uid="{43E95DCD-632B-4918-A2CA-0F08DDA5C566}"/>
+    <hyperlink ref="D65" r:id="rId6" xr:uid="{E9A61742-5A22-43CC-A706-547AA7FF8BAB}"/>
+    <hyperlink ref="D77" r:id="rId7" xr:uid="{B29F2E94-69AB-436A-8A88-9A5368167FD7}"/>
+    <hyperlink ref="D89" r:id="rId8" xr:uid="{98873325-DEA6-43F9-91A0-E8FB4B8A97A0}"/>
+    <hyperlink ref="D101" r:id="rId9" xr:uid="{E6AE0669-60C4-406B-A1CE-3157C24E4D86}"/>
+    <hyperlink ref="D113" r:id="rId10" xr:uid="{C663B635-A303-436B-A6A0-DBFC03C0AAA2}"/>
+    <hyperlink ref="D125" r:id="rId11" xr:uid="{A90620B7-DD2E-4A8D-8B69-A69813292DFF}"/>
+    <hyperlink ref="D161" r:id="rId12" xr:uid="{3E73A8AF-10D6-4514-BE74-8DA1C314FA5C}"/>
+    <hyperlink ref="D137" r:id="rId13" xr:uid="{C44FB350-7347-420F-B32E-FF48994E370D}"/>
+    <hyperlink ref="D149" r:id="rId14" xr:uid="{816EEEF3-3B4A-486F-A339-559F5C8C790A}"/>
+    <hyperlink ref="D173" r:id="rId15" xr:uid="{9CC31E5A-F3E9-4C7A-AF69-822FDCBCB956}"/>
+    <hyperlink ref="D185" r:id="rId16" xr:uid="{373F031B-BE99-409D-8449-FE1960BE5AAD}"/>
+    <hyperlink ref="D197" r:id="rId17" xr:uid="{DDD8C2D6-8779-49E8-B57E-B1CD776932DF}"/>
+    <hyperlink ref="D209" r:id="rId18" xr:uid="{269E504D-ED0F-44F0-82E7-CD2DDAD8785E}"/>
+    <hyperlink ref="D221" r:id="rId19" xr:uid="{E4CE4C6B-90D7-4BE7-8BC7-234EB03AA6CC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>